<commit_message>
created combined soil data file
</commit_message>
<xml_diff>
--- a/01_input/Data_microbial_biomass_BT_Janina_Hämmerli.xlsx
+++ b/01_input/Data_microbial_biomass_BT_Janina_Hämmerli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f304f79f068e311c/Universitaet/MASTER/MasterThesis/11_Data_Analysis_MA/01_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_E5F59D3EF76A2DC85E421D1BC41EE535EDA5537A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BCFEECC-CB30-4DED-A543-07EBAD9E0011}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_E5F59D3EF76A2DC85E421D1BC41EE535EDA5537A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9E4DD64-2822-4C35-82A3-3E6D68344AD7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="60855" yWindow="3255" windowWidth="14160" windowHeight="7170" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59760" yWindow="2160" windowWidth="21600" windowHeight="12150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Janina Hämmerli 29_05_2024 08-3" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6834" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6834" uniqueCount="586">
   <si>
     <t>#DIMAQS CSV EXPORT 5.1.41.32 23/09/2020</t>
   </si>
@@ -1802,6 +1802,9 @@
   </si>
   <si>
     <t>Standart deviations</t>
+  </si>
+  <si>
+    <t>2_1_2</t>
   </si>
 </sst>
 </file>
@@ -43933,8 +43936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -43985,7 +43988,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>543</v>
+        <v>585</v>
       </c>
       <c r="B6">
         <v>424.74731590352593</v>
@@ -44219,7 +44222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>

</xml_diff>